<commit_message>
feat: complete read api for entities
</commit_message>
<xml_diff>
--- a/Documents/it_services_connection.xlsx
+++ b/Documents/it_services_connection.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Service" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="GroupModule" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Instance" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Server" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Module" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="Database" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="Storage" sheetId="6" state="visible" r:id="rId8"/>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">Processes</t>
   </si>
   <si>
-    <t xml:space="preserve">instance_ip</t>
+    <t xml:space="preserve">server_ip</t>
   </si>
   <si>
     <t xml:space="preserve">10.0.1.11</t>
@@ -182,7 +182,7 @@
     <t xml:space="preserve">group_module_id</t>
   </si>
   <si>
-    <t xml:space="preserve">instance_id</t>
+    <t xml:space="preserve">server_id</t>
   </si>
   <si>
     <t xml:space="preserve">module_code</t>
@@ -591,16 +591,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -798,80 +802,80 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -899,176 +903,176 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="B5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="B6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" s="0" t="s">
+      <c r="B7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="0" t="s">
+      <c r="B10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="B11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1091,204 +1095,204 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1310,535 +1314,535 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="B5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="0" t="n">
+      <c r="B6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="C7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" s="0" t="s">
+      <c r="C8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="B9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" s="0" t="n">
+      <c r="B10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="C11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D12" s="0" t="n">
+      <c r="C12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D13" s="0" t="n">
+      <c r="C13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="C14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C15" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D15" s="0" t="n">
+      <c r="C15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D16" s="0" t="n">
+      <c r="C16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C17" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D17" s="0" t="n">
+      <c r="C17" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C18" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D18" s="0" t="n">
+      <c r="C18" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C19" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D19" s="0" t="n">
+      <c r="C19" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C20" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D20" s="0" t="n">
+      <c r="C20" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" s="1" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1861,201 +1865,201 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>4</v>
       </c>
     </row>
@@ -2078,168 +2082,168 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>23</v>
       </c>
     </row>
@@ -2267,506 +2271,506 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="A7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="0" t="s">
+      <c r="C7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>8080</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" s="0" t="n">
+      <c r="A8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" s="0" t="s">
+      <c r="C8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>8080</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B9" s="0" t="n">
+      <c r="A9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="0" t="s">
+      <c r="C9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>8080</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" s="0" t="s">
+      <c r="C10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>8080</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>9000</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>9000</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D13" s="0" t="s">
+      <c r="B13" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>5432</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>5432</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>5432</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>5432</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>5432</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>5432</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <v>5432</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="1" t="n">
         <v>5432</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="1" t="n">
         <v>9443</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="1" t="n">
         <v>9443</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="1" t="n">
         <v>5432</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="G23" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="1" t="n">
         <v>5432</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="1" t="n">
         <v>5432</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="1" t="n">
         <v>5432</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="1" t="n">
         <v>5432</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2794,73 +2798,73 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>9000</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>9443</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>